<commit_message>
add more analysis details to xlsx file
</commit_message>
<xml_diff>
--- a/files_to_evaluate_quiet_061920.xlsx
+++ b/files_to_evaluate_quiet_061920.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfomac/github/dfo/anthropause/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{912EEB94-939E-9D46-B5FD-36A32C052FFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7CA6B7-DB96-AF4E-94A0-3B9197DCD602}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14200" yWindow="460" windowWidth="14600" windowHeight="16040" activeTab="1"/>
+    <workbookView xWindow="-47800" yWindow="6000" windowWidth="23000" windowHeight="16980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="files_to_evaluate_quiet_061920" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="99">
   <si>
     <t>inter</t>
   </si>
@@ -293,12 +293,48 @@
   </si>
   <si>
     <t>PE_completed</t>
+  </si>
+  <si>
+    <t>increment</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>configure view axes</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>15 sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">position </t>
+  </si>
+  <si>
+    <t>1400 Hz</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Freq</t>
+  </si>
+  <si>
+    <t>20 Hz</t>
+  </si>
+  <si>
+    <t>focus</t>
+  </si>
+  <si>
+    <t>All saved as Use_fish_calls preset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1134,11 +1170,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1264,7 +1300,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ref="I4:I67" si="1">(H4*(60*30))+G4</f>
+        <f t="shared" ref="I4:I63" si="1">(H4*(60*30))+G4</f>
         <v>1653.0000998973851</v>
       </c>
     </row>
@@ -4400,11 +4436,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -5728,16 +5765,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -5745,7 +5782,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -5753,49 +5790,113 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>76</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>77</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>80</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>81</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>83</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
selection tables so far and update to file list and gitingnore
</commit_message>
<xml_diff>
--- a/files_to_evaluate_quiet_061920.xlsx
+++ b/files_to_evaluate_quiet_061920.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfomac/github/dfo/anthropause/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7CA6B7-DB96-AF4E-94A0-3B9197DCD602}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97EC61B-468A-EB45-A696-98B6339D9F30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-47800" yWindow="6000" windowWidth="23000" windowHeight="16980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="26280" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="files_to_evaluate_quiet_061920" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="100">
   <si>
     <t>inter</t>
   </si>
@@ -329,13 +329,19 @@
   </si>
   <si>
     <t>All saved as Use_fish_calls preset</t>
+  </si>
+  <si>
+    <t>turn brightness to 40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-1009]d/mmm/yy;@"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -466,6 +472,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -652,7 +664,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -767,6 +779,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -812,10 +833,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1173,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M73" sqref="M73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4442,10 +4467,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4453,8 +4481,8 @@
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -4470,10 +4498,10 @@
       <c r="D1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>86</v>
       </c>
       <c r="G1" t="s">
@@ -4493,6 +4521,9 @@
       <c r="D2" s="2">
         <v>1201.0000998973801</v>
       </c>
+      <c r="F2" s="3">
+        <v>44092</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -4535,6 +4566,9 @@
       <c r="D5" s="2">
         <v>6961.0000998973801</v>
       </c>
+      <c r="F5" s="3">
+        <v>44092</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -4544,10 +4578,10 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
-        <v>6961.0000998973846</v>
+        <v>8372.000099897381</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4558,10 +4592,10 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2">
-        <v>8372.000099897381</v>
+        <v>10081.000099897381</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -4569,13 +4603,19 @@
         <v>2019</v>
       </c>
       <c r="B8">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D8" s="2">
-        <v>10081.000099897381</v>
+        <v>11101.000099897385</v>
+      </c>
+      <c r="E8" s="3">
+        <v>44091</v>
+      </c>
+      <c r="F8" s="3">
+        <v>44091</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -4586,10 +4626,10 @@
         <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2">
-        <v>11101.000099897385</v>
+        <v>12324</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -4600,10 +4640,10 @@
         <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2">
-        <v>12324</v>
+        <v>13561.000099897385</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -4611,13 +4651,13 @@
         <v>2019</v>
       </c>
       <c r="B11">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D11" s="2">
-        <v>13561.000099897385</v>
+        <v>15058.999900102615</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -4628,10 +4668,10 @@
         <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D12" s="2">
-        <v>15058.999900102615</v>
+        <v>15430.999900102619</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -4642,10 +4682,10 @@
         <v>89</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2">
-        <v>15430.999900102619</v>
+        <v>16140</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -4653,13 +4693,13 @@
         <v>2019</v>
       </c>
       <c r="B14">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D14" s="2">
-        <v>16140</v>
+        <v>18721.000099897385</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -4670,10 +4710,10 @@
         <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D15" s="2">
-        <v>18721.000099897385</v>
+        <v>19096</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -4684,10 +4724,10 @@
         <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D16" s="2">
-        <v>19096</v>
+        <v>19860</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -4695,13 +4735,13 @@
         <v>2019</v>
       </c>
       <c r="B17">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D17" s="2">
-        <v>19860</v>
+        <v>21900</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -4712,10 +4752,10 @@
         <v>105</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D18" s="2">
-        <v>21900</v>
+        <v>22334</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -4726,10 +4766,10 @@
         <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2">
-        <v>22334</v>
+        <v>22981.000099897381</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -4737,13 +4777,13 @@
         <v>2019</v>
       </c>
       <c r="B20">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D20" s="2">
-        <v>22981.000099897381</v>
+        <v>25081.000099897381</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -4757,7 +4797,7 @@
         <v>6</v>
       </c>
       <c r="D21" s="2">
-        <v>25081.000099897381</v>
+        <v>25081.000099897385</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -4768,10 +4808,10 @@
         <v>107</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D22" s="2">
-        <v>25081.000099897385</v>
+        <v>25842.000099897385</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -4782,10 +4822,10 @@
         <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D23" s="2">
-        <v>25842.000099897385</v>
+        <v>26521.000099897381</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -4793,13 +4833,13 @@
         <v>2019</v>
       </c>
       <c r="B24">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D24" s="2">
-        <v>26521.000099897381</v>
+        <v>27121.000099897385</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -4810,10 +4850,10 @@
         <v>109</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D25" s="2">
-        <v>27121.000099897385</v>
+        <v>27550.000099897385</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -4824,10 +4864,10 @@
         <v>109</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D26" s="2">
-        <v>27550.000099897385</v>
+        <v>28321.000099897381</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -4835,13 +4875,13 @@
         <v>2019</v>
       </c>
       <c r="B27">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D27" s="2">
-        <v>28321.000099897381</v>
+        <v>29041.000099897385</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -4852,10 +4892,10 @@
         <v>111</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D28" s="2">
-        <v>29041.000099897385</v>
+        <v>29383.000099897385</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -4866,10 +4906,10 @@
         <v>111</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D29" s="2">
-        <v>29383.000099897385</v>
+        <v>30121.000099897381</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -4877,13 +4917,13 @@
         <v>2019</v>
       </c>
       <c r="B30">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D30" s="2">
-        <v>30121.000099897381</v>
+        <v>32281.000099897381</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -4894,10 +4934,10 @@
         <v>113</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D31" s="2">
-        <v>32281.000099897381</v>
+        <v>32640</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -4908,10 +4948,10 @@
         <v>113</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D32" s="2">
-        <v>32640</v>
+        <v>33721.000099897377</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -4919,13 +4959,13 @@
         <v>2019</v>
       </c>
       <c r="B33">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D33" s="2">
-        <v>33721.000099897377</v>
+        <v>35762.000199794769</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -4936,10 +4976,10 @@
         <v>115</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D34" s="2">
-        <v>35762.000199794769</v>
+        <v>36235.000099897385</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -4950,10 +4990,10 @@
         <v>115</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D35" s="2">
-        <v>36235.000099897385</v>
+        <v>36901.000099897385</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -4961,13 +5001,13 @@
         <v>2019</v>
       </c>
       <c r="B36">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D36" s="2">
-        <v>36901.000099897385</v>
+        <v>38040</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -4978,10 +5018,10 @@
         <v>117</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D37" s="2">
-        <v>38040</v>
+        <v>38499</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -4992,10 +5032,10 @@
         <v>117</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D38" s="2">
-        <v>38499</v>
+        <v>39600</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -5003,13 +5043,13 @@
         <v>2019</v>
       </c>
       <c r="B39">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D39" s="2">
-        <v>39600</v>
+        <v>42721.000099897377</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -5020,10 +5060,10 @@
         <v>125</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D40" s="2">
-        <v>42721.000099897377</v>
+        <v>43730</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -5034,10 +5074,10 @@
         <v>125</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D41" s="2">
-        <v>43730</v>
+        <v>44401.000099897377</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -5045,13 +5085,13 @@
         <v>2019</v>
       </c>
       <c r="B42">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D42" s="2">
-        <v>44401.000099897377</v>
+        <v>45061.000099897385</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -5062,10 +5102,10 @@
         <v>129</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D43" s="2">
-        <v>45061.000099897385</v>
+        <v>45835.000099897385</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -5076,10 +5116,10 @@
         <v>129</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D44" s="2">
-        <v>45835.000099897385</v>
+        <v>46321.000099897377</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -5087,13 +5127,13 @@
         <v>2019</v>
       </c>
       <c r="B45">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D45" s="2">
-        <v>46321.000099897377</v>
+        <v>47100</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -5104,10 +5144,10 @@
         <v>133</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D46" s="2">
-        <v>47100</v>
+        <v>47457.999900102615</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -5118,10 +5158,10 @@
         <v>133</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D47" s="2">
-        <v>47457.999900102615</v>
+        <v>48600</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -5129,16 +5169,16 @@
         <v>2019</v>
       </c>
       <c r="B48">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C48" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D48" s="2">
-        <v>48600</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>50760</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2019</v>
       </c>
@@ -5146,13 +5186,13 @@
         <v>141</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D49" s="2">
-        <v>50760</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>51789</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2019</v>
       </c>
@@ -5160,27 +5200,27 @@
         <v>141</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D50" s="2">
-        <v>51789</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>52500</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2019</v>
       </c>
       <c r="B51">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D51" s="2">
-        <v>52500</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>55141.000099897377</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2019</v>
       </c>
@@ -5188,13 +5228,13 @@
         <v>151</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D52" s="2">
-        <v>55141.000099897377</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>55478.000099897377</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2019</v>
       </c>
@@ -5202,27 +5242,27 @@
         <v>151</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D53" s="2">
-        <v>55478.000099897377</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>56941.000099897377</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2019</v>
       </c>
       <c r="B54">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C54" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D54" s="2">
-        <v>56941.000099897377</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>57721.000099897385</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2019</v>
       </c>
@@ -5230,13 +5270,13 @@
         <v>155</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D55" s="2">
-        <v>57721.000099897385</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+        <v>58069.000099897385</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2019</v>
       </c>
@@ -5244,27 +5284,34 @@
         <v>155</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D56" s="2">
-        <v>58069.000099897385</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>2019</v>
-      </c>
-      <c r="B57">
-        <v>155</v>
-      </c>
-      <c r="C57" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" s="2">
         <v>58801.000099897377</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="4">
+        <v>2020</v>
+      </c>
+      <c r="B57" s="4">
+        <v>207</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="5">
+        <v>661.00009989738498</v>
+      </c>
+      <c r="E57" s="6"/>
+      <c r="F57" s="3">
+        <v>44092</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2020</v>
       </c>
@@ -5272,13 +5319,13 @@
         <v>207</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D58" s="2">
-        <v>661.00009989738498</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2020</v>
       </c>
@@ -5286,27 +5333,30 @@
         <v>207</v>
       </c>
       <c r="C59" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D59" s="2">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2020</v>
       </c>
       <c r="B60">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D60" s="2">
-        <v>1860</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3180</v>
+      </c>
+      <c r="F60" s="3">
+        <v>44092</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2020</v>
       </c>
@@ -5314,13 +5364,13 @@
         <v>209</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D61" s="2">
-        <v>3180</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3523</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2020</v>
       </c>
@@ -5328,27 +5378,30 @@
         <v>209</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D62" s="2">
-        <v>3523</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2020</v>
       </c>
       <c r="B63">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C63" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D63" s="2">
-        <v>4560</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5940</v>
+      </c>
+      <c r="F63" s="3">
+        <v>44092</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2020</v>
       </c>
@@ -5356,10 +5409,10 @@
         <v>211</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D64" s="2">
-        <v>5940</v>
+        <v>6913</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -5370,10 +5423,10 @@
         <v>211</v>
       </c>
       <c r="C65" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D65" s="2">
-        <v>6913</v>
+        <v>7260</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -5381,13 +5434,13 @@
         <v>2020</v>
       </c>
       <c r="B66">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C66" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D66" s="2">
-        <v>7260</v>
+        <v>8820</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -5398,10 +5451,10 @@
         <v>213</v>
       </c>
       <c r="C67" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D67" s="2">
-        <v>8820</v>
+        <v>9425</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -5412,10 +5465,10 @@
         <v>213</v>
       </c>
       <c r="C68" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D68" s="2">
-        <v>9425</v>
+        <v>9960</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -5423,13 +5476,13 @@
         <v>2020</v>
       </c>
       <c r="B69">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C69" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D69" s="2">
-        <v>9960</v>
+        <v>10798.999900102615</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -5440,10 +5493,10 @@
         <v>215</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D70" s="2">
-        <v>10798.999900102615</v>
+        <v>11106.999900102615</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -5454,10 +5507,10 @@
         <v>215</v>
       </c>
       <c r="C71" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D71" s="2">
-        <v>11106.999900102615</v>
+        <v>11760</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -5465,13 +5518,13 @@
         <v>2020</v>
       </c>
       <c r="B72">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D72" s="2">
-        <v>11760</v>
+        <v>13440</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -5482,10 +5535,10 @@
         <v>219</v>
       </c>
       <c r="C73" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D73" s="2">
-        <v>13440</v>
+        <v>13789</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -5496,10 +5549,10 @@
         <v>219</v>
       </c>
       <c r="C74" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D74" s="2">
-        <v>13789</v>
+        <v>14340</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -5507,13 +5560,13 @@
         <v>2020</v>
       </c>
       <c r="B75">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C75" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D75" s="2">
-        <v>14340</v>
+        <v>15360</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -5524,10 +5577,10 @@
         <v>223</v>
       </c>
       <c r="C76" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D76" s="2">
-        <v>15360</v>
+        <v>16248</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -5538,10 +5591,10 @@
         <v>223</v>
       </c>
       <c r="C77" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D77" s="2">
-        <v>16248</v>
+        <v>17340</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -5549,13 +5602,13 @@
         <v>2020</v>
       </c>
       <c r="B78">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C78" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D78" s="2">
-        <v>17340</v>
+        <v>18240</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -5566,10 +5619,10 @@
         <v>225</v>
       </c>
       <c r="C79" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D79" s="2">
-        <v>18240</v>
+        <v>18597</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -5580,10 +5633,10 @@
         <v>225</v>
       </c>
       <c r="C80" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D80" s="2">
-        <v>18597</v>
+        <v>18960</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -5591,13 +5644,13 @@
         <v>2020</v>
       </c>
       <c r="B81">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C81" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D81" s="2">
-        <v>18960</v>
+        <v>19980</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -5608,10 +5661,10 @@
         <v>229</v>
       </c>
       <c r="C82" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D82" s="2">
-        <v>19980</v>
+        <v>20330</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -5622,10 +5675,10 @@
         <v>229</v>
       </c>
       <c r="C83" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D83" s="2">
-        <v>20330</v>
+        <v>21181.000099897385</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -5633,13 +5686,13 @@
         <v>2020</v>
       </c>
       <c r="B84">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C84" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D84" s="2">
-        <v>21181.000099897385</v>
+        <v>22320</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -5650,10 +5703,10 @@
         <v>233</v>
       </c>
       <c r="C85" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D85" s="2">
-        <v>22320</v>
+        <v>22655</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -5664,10 +5717,10 @@
         <v>233</v>
       </c>
       <c r="C86" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D86" s="2">
-        <v>22655</v>
+        <v>23460</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -5675,13 +5728,13 @@
         <v>2020</v>
       </c>
       <c r="B87">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C87" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D87" s="2">
-        <v>23460</v>
+        <v>25080</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -5692,10 +5745,10 @@
         <v>235</v>
       </c>
       <c r="C88" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D88" s="2">
-        <v>25080</v>
+        <v>25437</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -5706,25 +5759,14 @@
         <v>235</v>
       </c>
       <c r="C89" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D89" s="2">
-        <v>25437</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>2020</v>
-      </c>
-      <c r="B90">
-        <v>235</v>
-      </c>
-      <c r="C90" t="s">
-        <v>10</v>
-      </c>
-      <c r="D90" s="2">
         <v>26280</v>
       </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D91"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D92"/>
@@ -5756,147 +5798,146 @@
     <row r="101" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D101"/>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D102"/>
-    </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B1">
-        <v>48</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B2">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B3">
-        <v>10500</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>79</v>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" t="s">
-        <v>82</v>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B10">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>75</v>
+      </c>
+      <c r="B12">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>94</v>
-      </c>
-      <c r="C13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" t="s">
-        <v>91</v>
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13">
+        <v>10500</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" t="s">
-        <v>96</v>
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>80</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>